<commit_message>
added Readme for eda
</commit_message>
<xml_diff>
--- a/EDA Project /auction_summer.xlsx
+++ b/EDA Project /auction_summer.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28209"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28908"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tomasespina/Desktop/ThinkFul Python/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tomasespina/Desktop/K2 Data Science/Repo/EDA Project /"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -146,9 +146,6 @@
     <t>Appraisal</t>
   </si>
   <si>
-    <t>MIn Bid</t>
-  </si>
-  <si>
     <t>Township</t>
   </si>
   <si>
@@ -1539,6 +1536,9 @@
   </si>
   <si>
     <t>7824 EUSTIS CT</t>
+  </si>
+  <si>
+    <t>Min Bid</t>
   </si>
 </sst>
 </file>
@@ -1883,7 +1883,7 @@
   <dimension ref="A1:K150"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A124" sqref="A124:K129"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1923,10 +1923,10 @@
         <v>38</v>
       </c>
       <c r="H1" s="4" t="s">
+        <v>503</v>
+      </c>
+      <c r="I1" s="4" t="s">
         <v>39</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>40</v>
       </c>
       <c r="J1" s="4" t="s">
         <v>4</v>
@@ -1937,19 +1937,19 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>34</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>66</v>
-      </c>
       <c r="E2" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>32</v>
@@ -1961,7 +1961,7 @@
         <v>56000</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J2" s="1"/>
       <c r="K2" s="3">
@@ -1970,16 +1970,16 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>69</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>70</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>11</v>
@@ -1994,7 +1994,7 @@
         <v>32000</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="J3" s="1"/>
       <c r="K3" s="3">
@@ -2003,16 +2003,16 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>23</v>
       </c>
       <c r="C4" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>73</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>74</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>18</v>
@@ -2027,7 +2027,7 @@
         <v>60000</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J4" s="1"/>
       <c r="K4" s="3">
@@ -2036,16 +2036,16 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C5" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>77</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>78</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>21</v>
@@ -2060,7 +2060,7 @@
         <v>50000</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J5" s="1"/>
       <c r="K5" s="3">
@@ -2069,16 +2069,16 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>23</v>
       </c>
       <c r="C6" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>80</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>81</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>18</v>
@@ -2093,7 +2093,7 @@
         <v>68000</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J6" s="1"/>
       <c r="K6" s="3">
@@ -2102,16 +2102,16 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C7" s="1" t="s">
+      <c r="D7" s="1" t="s">
         <v>84</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>85</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>21</v>
@@ -2126,7 +2126,7 @@
         <v>54000</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J7" s="1"/>
       <c r="K7" s="3">
@@ -2135,22 +2135,22 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="D8" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="E8" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C8" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="E8" s="1" t="s">
+      <c r="F8" s="1" t="s">
         <v>50</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>51</v>
       </c>
       <c r="G8" s="2">
         <v>60000</v>
@@ -2159,7 +2159,7 @@
         <v>40000</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="J8" s="1"/>
       <c r="K8" s="3">
@@ -2168,16 +2168,16 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>16</v>
       </c>
       <c r="C9" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="D9" s="1" t="s">
         <v>91</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>92</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>13</v>
@@ -2192,7 +2192,7 @@
         <v>26000</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J9" s="1"/>
       <c r="K9" s="3">
@@ -2201,19 +2201,19 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>16</v>
       </c>
       <c r="C10" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D10" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="D10" s="1" t="s">
-        <v>96</v>
-      </c>
       <c r="E10" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>32</v>
@@ -2225,7 +2225,7 @@
         <v>22000</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J10" s="1"/>
       <c r="K10" s="3">
@@ -2234,16 +2234,16 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C11" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="D11" s="1" t="s">
         <v>98</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>99</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>21</v>
@@ -2258,7 +2258,7 @@
         <v>100000</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="J11" s="1"/>
       <c r="K11" s="3">
@@ -2267,16 +2267,16 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C12" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="D12" s="1" t="s">
         <v>102</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>103</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>13</v>
@@ -2291,7 +2291,7 @@
         <v>108000</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J12" s="1"/>
       <c r="K12" s="3">
@@ -2300,16 +2300,16 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C13" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="D13" s="1" t="s">
         <v>105</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>106</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>13</v>
@@ -2324,7 +2324,7 @@
         <v>68000</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J13" s="1"/>
       <c r="K13" s="3">
@@ -2333,22 +2333,22 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="C14" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="D14" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="E14" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="E14" s="1" t="s">
+      <c r="F14" s="1" t="s">
         <v>111</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>112</v>
       </c>
       <c r="G14" s="2">
         <v>147000</v>
@@ -2357,7 +2357,7 @@
         <v>98000</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J14" s="1"/>
       <c r="K14" s="3">
@@ -2366,16 +2366,16 @@
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C15" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="B15" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C15" s="1" t="s">
+      <c r="D15" s="1" t="s">
         <v>114</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>115</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>21</v>
@@ -2390,7 +2390,7 @@
         <v>54000</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="J15" s="1"/>
       <c r="K15" s="3">
@@ -2399,22 +2399,22 @@
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C16" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="D16" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="E16" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="C16" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="E16" s="1" t="s">
+      <c r="F16" s="1" t="s">
         <v>54</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>55</v>
       </c>
       <c r="G16" s="2">
         <v>54000</v>
@@ -2423,7 +2423,7 @@
         <v>36000</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J16" s="1"/>
       <c r="K16" s="3">
@@ -2432,19 +2432,19 @@
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B17" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="C17" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="D17" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="D17" s="1" t="s">
-        <v>123</v>
-      </c>
       <c r="E17" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F17" s="1" t="s">
         <v>32</v>
@@ -2456,7 +2456,7 @@
         <v>42000</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J17" s="1"/>
       <c r="K17" s="3">
@@ -2465,16 +2465,16 @@
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>20</v>
       </c>
       <c r="C18" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="D18" s="1" t="s">
         <v>125</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>126</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>21</v>
@@ -2489,7 +2489,7 @@
         <v>5400</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J18" s="1"/>
       <c r="K18" s="3">
@@ -2498,16 +2498,16 @@
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B19" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="C19" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="D19" s="1" t="s">
         <v>129</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>130</v>
       </c>
       <c r="E19" s="1" t="s">
         <v>13</v>
@@ -2522,7 +2522,7 @@
         <v>56000</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J19" s="1"/>
       <c r="K19" s="3">
@@ -2531,16 +2531,16 @@
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C20" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="D20" s="1" t="s">
         <v>132</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>133</v>
       </c>
       <c r="E20" s="1" t="s">
         <v>13</v>
@@ -2555,7 +2555,7 @@
         <v>76000</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="J20" s="1"/>
       <c r="K20" s="3">
@@ -2564,16 +2564,16 @@
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C21" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="B21" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C21" s="1" t="s">
+      <c r="D21" s="1" t="s">
         <v>135</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>136</v>
       </c>
       <c r="E21" s="1" t="s">
         <v>21</v>
@@ -2588,7 +2588,7 @@
         <v>28000</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="J21" s="1"/>
       <c r="K21" s="3">
@@ -2597,16 +2597,16 @@
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C22" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="B22" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C22" s="1" t="s">
+      <c r="D22" s="1" t="s">
         <v>139</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>140</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>21</v>
@@ -2621,7 +2621,7 @@
         <v>50000</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="J22" s="1"/>
       <c r="K22" s="3">
@@ -2630,16 +2630,16 @@
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="B23" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="C23" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="C23" s="1" t="s">
+      <c r="D23" s="1" t="s">
         <v>144</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>145</v>
       </c>
       <c r="E23" s="1" t="s">
         <v>21</v>
@@ -2654,7 +2654,7 @@
         <v>72000</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="J23" s="1"/>
       <c r="K23" s="3">
@@ -2663,16 +2663,16 @@
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C24" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="D24" s="1" t="s">
         <v>148</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>149</v>
       </c>
       <c r="E24" s="1" t="s">
         <v>13</v>
@@ -2687,7 +2687,7 @@
         <v>70000</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J24" s="1"/>
       <c r="K24" s="3">
@@ -2696,22 +2696,22 @@
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C25" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="D25" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="D25" s="1" t="s">
-        <v>152</v>
-      </c>
       <c r="E25" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="F25" s="1" t="s">
         <v>50</v>
-      </c>
-      <c r="F25" s="1" t="s">
-        <v>51</v>
       </c>
       <c r="G25" s="2">
         <v>75000</v>
@@ -2720,7 +2720,7 @@
         <v>50000</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="J25" s="1"/>
       <c r="K25" s="3">
@@ -2729,22 +2729,22 @@
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C26" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="D26" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="D26" s="1" t="s">
-        <v>155</v>
-      </c>
       <c r="E26" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="F26" s="1" t="s">
         <v>50</v>
-      </c>
-      <c r="F26" s="1" t="s">
-        <v>51</v>
       </c>
       <c r="G26" s="2">
         <v>45000</v>
@@ -2753,7 +2753,7 @@
         <v>30000</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="J26" s="1"/>
       <c r="K26" s="3">
@@ -2762,16 +2762,16 @@
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>24</v>
       </c>
       <c r="C27" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="D27" s="1" t="s">
         <v>157</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>158</v>
       </c>
       <c r="E27" s="1" t="s">
         <v>13</v>
@@ -2786,7 +2786,7 @@
         <v>132000</v>
       </c>
       <c r="I27" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J27" s="1"/>
       <c r="K27" s="3">
@@ -2795,16 +2795,16 @@
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>33</v>
       </c>
       <c r="C28" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="D28" s="1" t="s">
         <v>374</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>375</v>
       </c>
       <c r="E28" s="1" t="s">
         <v>13</v>
@@ -2819,7 +2819,7 @@
         <v>252000</v>
       </c>
       <c r="I28" s="1" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="J28" s="1"/>
       <c r="K28" s="3">
@@ -2828,22 +2828,22 @@
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C29" s="1" t="s">
+        <v>377</v>
+      </c>
+      <c r="D29" s="1" t="s">
         <v>378</v>
       </c>
-      <c r="D29" s="1" t="s">
+      <c r="E29" s="1" t="s">
         <v>379</v>
       </c>
-      <c r="E29" s="1" t="s">
+      <c r="F29" s="1" t="s">
         <v>380</v>
-      </c>
-      <c r="F29" s="1" t="s">
-        <v>381</v>
       </c>
       <c r="G29" s="2">
         <v>75000</v>
@@ -2852,7 +2852,7 @@
         <v>50000</v>
       </c>
       <c r="I29" s="1" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="J29" s="1"/>
       <c r="K29" s="3">
@@ -2861,16 +2861,16 @@
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C30" s="1" t="s">
+        <v>383</v>
+      </c>
+      <c r="D30" s="1" t="s">
         <v>384</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>385</v>
       </c>
       <c r="E30" s="1" t="s">
         <v>21</v>
@@ -2885,7 +2885,7 @@
         <v>26000</v>
       </c>
       <c r="I30" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J30" s="1"/>
       <c r="K30" s="3">
@@ -2894,29 +2894,29 @@
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
+        <v>385</v>
+      </c>
+      <c r="B31" s="1" t="s">
         <v>386</v>
       </c>
-      <c r="B31" s="1" t="s">
+      <c r="C31" s="1" t="s">
         <v>387</v>
       </c>
-      <c r="C31" s="1" t="s">
+      <c r="D31" s="1" t="s">
         <v>388</v>
       </c>
-      <c r="D31" s="1" t="s">
+      <c r="E31" s="1" t="s">
         <v>389</v>
       </c>
-      <c r="E31" s="1" t="s">
+      <c r="F31" s="1" t="s">
         <v>390</v>
-      </c>
-      <c r="F31" s="1" t="s">
-        <v>391</v>
       </c>
       <c r="G31" s="1"/>
       <c r="H31" s="2">
         <v>600000</v>
       </c>
       <c r="I31" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="J31" s="1"/>
       <c r="K31" s="3">
@@ -2925,16 +2925,16 @@
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C32" s="1" t="s">
+        <v>392</v>
+      </c>
+      <c r="D32" s="1" t="s">
         <v>393</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>394</v>
       </c>
       <c r="E32" s="1" t="s">
         <v>21</v>
@@ -2949,7 +2949,7 @@
         <v>26000</v>
       </c>
       <c r="I32" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J32" s="1"/>
       <c r="K32" s="3">
@@ -2958,22 +2958,22 @@
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
+        <v>394</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C33" s="1" t="s">
         <v>395</v>
       </c>
-      <c r="B33" s="1" t="s">
+      <c r="D33" s="1" t="s">
+        <v>396</v>
+      </c>
+      <c r="E33" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C33" s="1" t="s">
-        <v>396</v>
-      </c>
-      <c r="D33" s="1" t="s">
-        <v>397</v>
-      </c>
-      <c r="E33" s="1" t="s">
+      <c r="F33" s="1" t="s">
         <v>46</v>
-      </c>
-      <c r="F33" s="1" t="s">
-        <v>47</v>
       </c>
       <c r="G33" s="2">
         <v>135000</v>
@@ -2982,7 +2982,7 @@
         <v>90000</v>
       </c>
       <c r="I33" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J33" s="1"/>
       <c r="K33" s="3">
@@ -2991,16 +2991,16 @@
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C34" s="1" t="s">
+        <v>398</v>
+      </c>
+      <c r="D34" s="1" t="s">
         <v>399</v>
-      </c>
-      <c r="D34" s="1" t="s">
-        <v>400</v>
       </c>
       <c r="E34" s="1" t="s">
         <v>11</v>
@@ -3015,7 +3015,7 @@
         <v>36000</v>
       </c>
       <c r="I34" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="J34" s="1"/>
       <c r="K34" s="3">
@@ -3024,16 +3024,16 @@
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="B35" s="1" t="s">
         <v>308</v>
       </c>
-      <c r="B35" s="1" t="s">
-        <v>309</v>
-      </c>
       <c r="C35" s="1" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="E35" s="1" t="s">
         <v>13</v>
@@ -3048,7 +3048,7 @@
         <v>42000</v>
       </c>
       <c r="I35" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J35" s="1"/>
       <c r="K35" s="3">
@@ -3057,16 +3057,16 @@
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C36" s="1" t="s">
+        <v>402</v>
+      </c>
+      <c r="D36" s="1" t="s">
         <v>403</v>
-      </c>
-      <c r="D36" s="1" t="s">
-        <v>404</v>
       </c>
       <c r="E36" s="1" t="s">
         <v>13</v>
@@ -3081,7 +3081,7 @@
         <v>62000</v>
       </c>
       <c r="I36" s="1" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="J36" s="1"/>
       <c r="K36" s="3">
@@ -3090,16 +3090,16 @@
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>34</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="E37" s="1" t="s">
         <v>21</v>
@@ -3114,7 +3114,7 @@
         <v>54000</v>
       </c>
       <c r="I37" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J37" s="1"/>
       <c r="K37" s="3">
@@ -3123,16 +3123,16 @@
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C38" s="1" t="s">
+        <v>407</v>
+      </c>
+      <c r="D38" s="1" t="s">
         <v>408</v>
-      </c>
-      <c r="D38" s="1" t="s">
-        <v>409</v>
       </c>
       <c r="E38" s="1" t="s">
         <v>13</v>
@@ -3147,7 +3147,7 @@
         <v>48000</v>
       </c>
       <c r="I38" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="J38" s="1"/>
       <c r="K38" s="3">
@@ -3156,16 +3156,16 @@
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
+        <v>409</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="C39" s="1" t="s">
         <v>410</v>
       </c>
-      <c r="B39" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="C39" s="1" t="s">
+      <c r="D39" s="1" t="s">
         <v>411</v>
-      </c>
-      <c r="D39" s="1" t="s">
-        <v>412</v>
       </c>
       <c r="E39" s="1" t="s">
         <v>25</v>
@@ -3180,7 +3180,7 @@
         <v>86000</v>
       </c>
       <c r="I39" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="J39" s="1"/>
       <c r="K39" s="3">
@@ -3189,16 +3189,16 @@
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
+        <v>412</v>
+      </c>
+      <c r="B40" s="1" t="s">
         <v>413</v>
       </c>
-      <c r="B40" s="1" t="s">
+      <c r="C40" s="1" t="s">
         <v>414</v>
       </c>
-      <c r="C40" s="1" t="s">
+      <c r="D40" s="1" t="s">
         <v>415</v>
-      </c>
-      <c r="D40" s="1" t="s">
-        <v>416</v>
       </c>
       <c r="E40" s="1" t="s">
         <v>21</v>
@@ -3213,7 +3213,7 @@
         <v>22000</v>
       </c>
       <c r="I40" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="J40" s="1"/>
       <c r="K40" s="3">
@@ -3222,16 +3222,16 @@
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C41" s="1" t="s">
+        <v>417</v>
+      </c>
+      <c r="D41" s="1" t="s">
         <v>418</v>
-      </c>
-      <c r="D41" s="1" t="s">
-        <v>419</v>
       </c>
       <c r="E41" s="1" t="s">
         <v>21</v>
@@ -3246,7 +3246,7 @@
         <v>82000</v>
       </c>
       <c r="I41" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J41" s="1"/>
       <c r="K41" s="3">
@@ -3255,16 +3255,16 @@
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="B42" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="E42" s="1" t="s">
         <v>8</v>
@@ -3279,7 +3279,7 @@
         <v>72000</v>
       </c>
       <c r="I42" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J42" s="1"/>
       <c r="K42" s="3">
@@ -3288,16 +3288,16 @@
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="B43" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C43" s="1" t="s">
+        <v>422</v>
+      </c>
+      <c r="D43" s="1" t="s">
         <v>423</v>
-      </c>
-      <c r="D43" s="1" t="s">
-        <v>424</v>
       </c>
       <c r="E43" s="1" t="s">
         <v>11</v>
@@ -3312,7 +3312,7 @@
         <v>50000</v>
       </c>
       <c r="I43" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J43" s="1"/>
       <c r="K43" s="3">
@@ -3321,16 +3321,16 @@
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="B44" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C44" s="1" t="s">
+        <v>425</v>
+      </c>
+      <c r="D44" s="1" t="s">
         <v>426</v>
-      </c>
-      <c r="D44" s="1" t="s">
-        <v>427</v>
       </c>
       <c r="E44" s="1" t="s">
         <v>8</v>
@@ -3345,7 +3345,7 @@
         <v>50000</v>
       </c>
       <c r="I44" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="J44" s="1"/>
       <c r="K44" s="3">
@@ -3354,16 +3354,16 @@
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="B45" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C45" s="1" t="s">
+        <v>428</v>
+      </c>
+      <c r="D45" s="1" t="s">
         <v>429</v>
-      </c>
-      <c r="D45" s="1" t="s">
-        <v>430</v>
       </c>
       <c r="E45" s="1" t="s">
         <v>21</v>
@@ -3378,7 +3378,7 @@
         <v>50000</v>
       </c>
       <c r="I45" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J45" s="1"/>
       <c r="K45" s="3">
@@ -3387,19 +3387,19 @@
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="B46" s="1" t="s">
         <v>33</v>
       </c>
       <c r="C46" s="1" t="s">
+        <v>431</v>
+      </c>
+      <c r="D46" s="1" t="s">
         <v>432</v>
       </c>
-      <c r="D46" s="1" t="s">
-        <v>433</v>
-      </c>
       <c r="E46" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F46" s="1" t="s">
         <v>32</v>
@@ -3411,7 +3411,7 @@
         <v>50000</v>
       </c>
       <c r="I46" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J46" s="1"/>
       <c r="K46" s="3">
@@ -3420,16 +3420,16 @@
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B47" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C47" s="1" t="s">
+        <v>434</v>
+      </c>
+      <c r="D47" s="1" t="s">
         <v>435</v>
-      </c>
-      <c r="D47" s="1" t="s">
-        <v>436</v>
       </c>
       <c r="E47" s="1" t="s">
         <v>18</v>
@@ -3444,7 +3444,7 @@
         <v>22000</v>
       </c>
       <c r="I47" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J47" s="1"/>
       <c r="K47" s="3">
@@ -3453,16 +3453,16 @@
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
+        <v>436</v>
+      </c>
+      <c r="B48" s="1" t="s">
         <v>437</v>
       </c>
-      <c r="B48" s="1" t="s">
+      <c r="C48" s="1" t="s">
         <v>438</v>
       </c>
-      <c r="C48" s="1" t="s">
+      <c r="D48" s="1" t="s">
         <v>439</v>
-      </c>
-      <c r="D48" s="1" t="s">
-        <v>440</v>
       </c>
       <c r="E48" s="1" t="s">
         <v>21</v>
@@ -3477,7 +3477,7 @@
         <v>60000</v>
       </c>
       <c r="I48" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J48" s="1"/>
       <c r="K48" s="3">
@@ -3486,19 +3486,19 @@
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="B49" s="1" t="s">
         <v>16</v>
       </c>
       <c r="C49" s="1" t="s">
+        <v>441</v>
+      </c>
+      <c r="D49" s="1" t="s">
         <v>442</v>
       </c>
-      <c r="D49" s="1" t="s">
-        <v>443</v>
-      </c>
       <c r="E49" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F49" s="1" t="s">
         <v>32</v>
@@ -3510,7 +3510,7 @@
         <v>32000</v>
       </c>
       <c r="I49" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J49" s="1"/>
       <c r="K49" s="3">
@@ -3519,16 +3519,16 @@
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="B50" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C50" s="1" t="s">
+        <v>444</v>
+      </c>
+      <c r="D50" s="1" t="s">
         <v>445</v>
-      </c>
-      <c r="D50" s="1" t="s">
-        <v>446</v>
       </c>
       <c r="E50" s="1" t="s">
         <v>21</v>
@@ -3543,7 +3543,7 @@
         <v>34000</v>
       </c>
       <c r="I50" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J50" s="1"/>
       <c r="K50" s="3">
@@ -3552,16 +3552,16 @@
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="B51" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C51" s="1" t="s">
+        <v>447</v>
+      </c>
+      <c r="D51" s="1" t="s">
         <v>448</v>
-      </c>
-      <c r="D51" s="1" t="s">
-        <v>449</v>
       </c>
       <c r="E51" s="1" t="s">
         <v>21</v>
@@ -3576,7 +3576,7 @@
         <v>88000</v>
       </c>
       <c r="I51" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="J51" s="1"/>
       <c r="K51" s="3">
@@ -3585,16 +3585,16 @@
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
+        <v>449</v>
+      </c>
+      <c r="B52" s="1" t="s">
         <v>450</v>
       </c>
-      <c r="B52" s="1" t="s">
+      <c r="C52" s="1" t="s">
         <v>451</v>
       </c>
-      <c r="C52" s="1" t="s">
+      <c r="D52" s="1" t="s">
         <v>452</v>
-      </c>
-      <c r="D52" s="1" t="s">
-        <v>453</v>
       </c>
       <c r="E52" s="1" t="s">
         <v>21</v>
@@ -3609,7 +3609,7 @@
         <v>72000</v>
       </c>
       <c r="I52" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="J52" s="1"/>
       <c r="K52" s="3">
@@ -3618,16 +3618,16 @@
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
+        <v>453</v>
+      </c>
+      <c r="B53" s="1" t="s">
         <v>454</v>
       </c>
-      <c r="B53" s="1" t="s">
+      <c r="C53" s="1" t="s">
         <v>455</v>
       </c>
-      <c r="C53" s="1" t="s">
+      <c r="D53" s="1" t="s">
         <v>456</v>
-      </c>
-      <c r="D53" s="1" t="s">
-        <v>457</v>
       </c>
       <c r="E53" s="1" t="s">
         <v>28</v>
@@ -3642,7 +3642,7 @@
         <v>48000</v>
       </c>
       <c r="I53" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J53" s="1"/>
       <c r="K53" s="3">
@@ -3651,22 +3651,22 @@
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
+        <v>457</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C54" s="1" t="s">
         <v>458</v>
       </c>
-      <c r="B54" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C54" s="1" t="s">
+      <c r="D54" s="1" t="s">
         <v>459</v>
       </c>
-      <c r="D54" s="1" t="s">
-        <v>460</v>
-      </c>
       <c r="E54" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="F54" s="1" t="s">
         <v>161</v>
-      </c>
-      <c r="F54" s="1" t="s">
-        <v>162</v>
       </c>
       <c r="G54" s="2">
         <v>54000</v>
@@ -3675,7 +3675,7 @@
         <v>36000</v>
       </c>
       <c r="I54" s="1" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="J54" s="1"/>
       <c r="K54" s="3">
@@ -3684,16 +3684,16 @@
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="B55" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C55" s="1" t="s">
+        <v>462</v>
+      </c>
+      <c r="D55" s="1" t="s">
         <v>463</v>
-      </c>
-      <c r="D55" s="1" t="s">
-        <v>464</v>
       </c>
       <c r="E55" s="1" t="s">
         <v>25</v>
@@ -3708,7 +3708,7 @@
         <v>2200</v>
       </c>
       <c r="I55" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J55" s="1"/>
       <c r="K55" s="3">
@@ -3717,16 +3717,16 @@
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="B56" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C56" s="1" t="s">
+        <v>465</v>
+      </c>
+      <c r="D56" s="1" t="s">
         <v>466</v>
-      </c>
-      <c r="D56" s="1" t="s">
-        <v>467</v>
       </c>
       <c r="E56" s="1" t="s">
         <v>8</v>
@@ -3741,7 +3741,7 @@
         <v>44000</v>
       </c>
       <c r="I56" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J56" s="1"/>
       <c r="K56" s="3">
@@ -3750,16 +3750,16 @@
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="B57" s="1" t="s">
         <v>23</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="E57" s="1" t="s">
         <v>18</v>
@@ -3774,7 +3774,7 @@
         <v>72000</v>
       </c>
       <c r="I57" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J57" s="1"/>
       <c r="K57" s="3">
@@ -3783,16 +3783,16 @@
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B58" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E58" s="1" t="s">
         <v>25</v>
@@ -3807,7 +3807,7 @@
         <v>18000</v>
       </c>
       <c r="I58" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J58" s="1"/>
       <c r="K58" s="3">
@@ -3816,22 +3816,22 @@
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B59" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="B59" s="1" t="s">
+      <c r="C59" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="C59" s="1" t="s">
+      <c r="D59" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="D59" s="1" t="s">
-        <v>172</v>
-      </c>
       <c r="E59" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="F59" s="1" t="s">
         <v>54</v>
-      </c>
-      <c r="F59" s="1" t="s">
-        <v>55</v>
       </c>
       <c r="G59" s="2">
         <v>153000</v>
@@ -3840,7 +3840,7 @@
         <v>102000</v>
       </c>
       <c r="I59" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J59" s="1"/>
       <c r="K59" s="3">
@@ -3849,16 +3849,16 @@
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="C60" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="B60" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="C60" s="1" t="s">
+      <c r="D60" s="1" t="s">
         <v>174</v>
-      </c>
-      <c r="D60" s="1" t="s">
-        <v>175</v>
       </c>
       <c r="E60" s="1" t="s">
         <v>21</v>
@@ -3873,7 +3873,7 @@
         <v>32000</v>
       </c>
       <c r="I60" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J60" s="1"/>
       <c r="K60" s="3">
@@ -3882,22 +3882,22 @@
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="B61" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="B61" s="1" t="s">
+      <c r="C61" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="C61" s="1" t="s">
+      <c r="D61" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="D61" s="1" t="s">
-        <v>179</v>
-      </c>
       <c r="E61" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="F61" s="1" t="s">
         <v>111</v>
-      </c>
-      <c r="F61" s="1" t="s">
-        <v>112</v>
       </c>
       <c r="G61" s="2">
         <v>96000</v>
@@ -3906,7 +3906,7 @@
         <v>64000</v>
       </c>
       <c r="I61" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J61" s="1"/>
       <c r="K61" s="3">
@@ -3915,19 +3915,19 @@
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B62" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C62" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="D62" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="D62" s="1" t="s">
-        <v>182</v>
-      </c>
       <c r="E62" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F62" s="1" t="s">
         <v>32</v>
@@ -3939,7 +3939,7 @@
         <v>12000</v>
       </c>
       <c r="I62" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="J62" s="1"/>
       <c r="K62" s="3">
@@ -3948,16 +3948,16 @@
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="B63" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="B63" s="1" t="s">
+      <c r="C63" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="C63" s="1" t="s">
+      <c r="D63" s="1" t="s">
         <v>186</v>
-      </c>
-      <c r="D63" s="1" t="s">
-        <v>187</v>
       </c>
       <c r="E63" s="1" t="s">
         <v>21</v>
@@ -3972,7 +3972,7 @@
         <v>48000</v>
       </c>
       <c r="I63" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="J63" s="1"/>
       <c r="K63" s="3">
@@ -3981,16 +3981,16 @@
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D64" s="1" t="s">
         <v>188</v>
-      </c>
-      <c r="B64" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C64" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="D64" s="1" t="s">
-        <v>189</v>
       </c>
       <c r="E64" s="1" t="s">
         <v>21</v>
@@ -4005,7 +4005,7 @@
         <v>38000</v>
       </c>
       <c r="I64" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="J64" s="1"/>
       <c r="K64" s="3">
@@ -4014,16 +4014,16 @@
     </row>
     <row r="65" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B65" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C65" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="D65" s="1" t="s">
         <v>191</v>
-      </c>
-      <c r="D65" s="1" t="s">
-        <v>192</v>
       </c>
       <c r="E65" s="1" t="s">
         <v>21</v>
@@ -4038,7 +4038,7 @@
         <v>32000</v>
       </c>
       <c r="I65" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="J65" s="1"/>
       <c r="K65" s="3">
@@ -4047,19 +4047,19 @@
     </row>
     <row r="66" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B66" s="1" t="s">
         <v>33</v>
       </c>
       <c r="C66" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="D66" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="D66" s="1" t="s">
-        <v>195</v>
-      </c>
       <c r="E66" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F66" s="1" t="s">
         <v>32</v>
@@ -4071,7 +4071,7 @@
         <v>44000</v>
       </c>
       <c r="I66" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J66" s="1"/>
       <c r="K66" s="3">
@@ -4080,16 +4080,16 @@
     </row>
     <row r="67" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B67" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C67" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="D67" s="1" t="s">
         <v>197</v>
-      </c>
-      <c r="D67" s="1" t="s">
-        <v>198</v>
       </c>
       <c r="E67" s="1" t="s">
         <v>21</v>
@@ -4104,7 +4104,7 @@
         <v>60000</v>
       </c>
       <c r="I67" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="J67" s="1"/>
       <c r="K67" s="3">
@@ -4113,16 +4113,16 @@
     </row>
     <row r="68" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C68" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="B68" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C68" s="1" t="s">
+      <c r="D68" s="1" t="s">
         <v>200</v>
-      </c>
-      <c r="D68" s="1" t="s">
-        <v>201</v>
       </c>
       <c r="E68" s="1" t="s">
         <v>21</v>
@@ -4137,7 +4137,7 @@
         <v>60000</v>
       </c>
       <c r="I68" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J68" s="1"/>
       <c r="K68" s="3">
@@ -4146,16 +4146,16 @@
     </row>
     <row r="69" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B69" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C69" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="D69" s="1" t="s">
         <v>203</v>
-      </c>
-      <c r="D69" s="1" t="s">
-        <v>204</v>
       </c>
       <c r="E69" s="1" t="s">
         <v>13</v>
@@ -4170,7 +4170,7 @@
         <v>22000</v>
       </c>
       <c r="I69" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="J69" s="1"/>
       <c r="K69" s="3">
@@ -4179,22 +4179,22 @@
     </row>
     <row r="70" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C70" s="1" t="s">
         <v>205</v>
       </c>
-      <c r="B70" s="1" t="s">
+      <c r="D70" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="E70" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C70" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="D70" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="E70" s="1" t="s">
+      <c r="F70" s="1" t="s">
         <v>46</v>
-      </c>
-      <c r="F70" s="1" t="s">
-        <v>47</v>
       </c>
       <c r="G70" s="2">
         <v>42000</v>
@@ -4203,7 +4203,7 @@
         <v>28000</v>
       </c>
       <c r="I70" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="J70" s="1"/>
       <c r="K70" s="3">
@@ -4212,16 +4212,16 @@
     </row>
     <row r="71" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B71" s="1" t="s">
         <v>31</v>
       </c>
       <c r="C71" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="D71" s="1" t="s">
         <v>209</v>
-      </c>
-      <c r="D71" s="1" t="s">
-        <v>210</v>
       </c>
       <c r="E71" s="1" t="s">
         <v>13</v>
@@ -4236,7 +4236,7 @@
         <v>28000</v>
       </c>
       <c r="I71" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="J71" s="1"/>
       <c r="K71" s="3">
@@ -4245,16 +4245,16 @@
     </row>
     <row r="72" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B72" s="1" t="s">
         <v>23</v>
       </c>
       <c r="C72" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="D72" s="1" t="s">
         <v>212</v>
-      </c>
-      <c r="D72" s="1" t="s">
-        <v>213</v>
       </c>
       <c r="E72" s="1" t="s">
         <v>18</v>
@@ -4269,7 +4269,7 @@
         <v>90000</v>
       </c>
       <c r="I72" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="J72" s="1"/>
       <c r="K72" s="3">
@@ -4278,16 +4278,16 @@
     </row>
     <row r="73" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="B73" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="B73" s="1" t="s">
+      <c r="C73" s="1" t="s">
         <v>215</v>
       </c>
-      <c r="C73" s="1" t="s">
+      <c r="D73" s="1" t="s">
         <v>216</v>
-      </c>
-      <c r="D73" s="1" t="s">
-        <v>217</v>
       </c>
       <c r="E73" s="1" t="s">
         <v>21</v>
@@ -4302,7 +4302,7 @@
         <v>170000</v>
       </c>
       <c r="I73" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="J73" s="1"/>
       <c r="K73" s="3">
@@ -4311,16 +4311,16 @@
     </row>
     <row r="74" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C74" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="B74" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C74" s="1" t="s">
-        <v>60</v>
-      </c>
       <c r="D74" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E74" s="1" t="s">
         <v>21</v>
@@ -4335,7 +4335,7 @@
         <v>36000</v>
       </c>
       <c r="I74" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="J74" s="1"/>
       <c r="K74" s="3">
@@ -4344,16 +4344,16 @@
     </row>
     <row r="75" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A75" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B75" s="1" t="s">
         <v>20</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E75" s="1" t="s">
         <v>21</v>
@@ -4368,7 +4368,7 @@
         <v>4000</v>
       </c>
       <c r="I75" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J75" s="1"/>
       <c r="K75" s="3">
@@ -4377,16 +4377,16 @@
     </row>
     <row r="76" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B76" s="1" t="s">
         <v>24</v>
       </c>
       <c r="C76" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="D76" s="1" t="s">
         <v>222</v>
-      </c>
-      <c r="D76" s="1" t="s">
-        <v>223</v>
       </c>
       <c r="E76" s="1" t="s">
         <v>21</v>
@@ -4401,7 +4401,7 @@
         <v>84000</v>
       </c>
       <c r="I76" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J76" s="1"/>
       <c r="K76" s="3">
@@ -4410,16 +4410,16 @@
     </row>
     <row r="77" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B77" s="1" t="s">
         <v>24</v>
       </c>
       <c r="C77" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="D77" s="1" t="s">
         <v>225</v>
-      </c>
-      <c r="D77" s="1" t="s">
-        <v>226</v>
       </c>
       <c r="E77" s="1" t="s">
         <v>11</v>
@@ -4434,7 +4434,7 @@
         <v>26000</v>
       </c>
       <c r="I77" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J77" s="1"/>
       <c r="K77" s="3">
@@ -4443,22 +4443,22 @@
     </row>
     <row r="78" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="B78" s="1" t="s">
         <v>227</v>
       </c>
-      <c r="B78" s="1" t="s">
+      <c r="C78" s="1" t="s">
         <v>228</v>
       </c>
-      <c r="C78" s="1" t="s">
+      <c r="D78" s="1" t="s">
         <v>229</v>
       </c>
-      <c r="D78" s="1" t="s">
-        <v>230</v>
-      </c>
       <c r="E78" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F78" s="1" t="s">
         <v>43</v>
-      </c>
-      <c r="F78" s="1" t="s">
-        <v>44</v>
       </c>
       <c r="G78" s="2">
         <v>120000</v>
@@ -4467,7 +4467,7 @@
         <v>80000</v>
       </c>
       <c r="I78" s="1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="J78" s="1"/>
       <c r="K78" s="3">
@@ -4476,22 +4476,22 @@
     </row>
     <row r="79" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B79" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C79" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="D79" s="1" t="s">
         <v>233</v>
       </c>
-      <c r="D79" s="1" t="s">
-        <v>234</v>
-      </c>
       <c r="E79" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="F79" s="1" t="s">
         <v>50</v>
-      </c>
-      <c r="F79" s="1" t="s">
-        <v>51</v>
       </c>
       <c r="G79" s="2">
         <v>3000</v>
@@ -4500,7 +4500,7 @@
         <v>2000</v>
       </c>
       <c r="I79" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J79" s="1"/>
       <c r="K79" s="3">
@@ -4509,16 +4509,16 @@
     </row>
     <row r="80" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="B80" s="1" t="s">
         <v>235</v>
       </c>
-      <c r="B80" s="1" t="s">
+      <c r="C80" s="1" t="s">
         <v>236</v>
       </c>
-      <c r="C80" s="1" t="s">
+      <c r="D80" s="1" t="s">
         <v>237</v>
-      </c>
-      <c r="D80" s="1" t="s">
-        <v>238</v>
       </c>
       <c r="E80" s="1" t="s">
         <v>28</v>
@@ -4533,7 +4533,7 @@
         <v>6000</v>
       </c>
       <c r="I80" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J80" s="1"/>
       <c r="K80" s="3">
@@ -4542,16 +4542,16 @@
     </row>
     <row r="81" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="B81" s="1" t="s">
         <v>239</v>
       </c>
-      <c r="B81" s="1" t="s">
+      <c r="C81" s="1" t="s">
         <v>240</v>
       </c>
-      <c r="C81" s="1" t="s">
+      <c r="D81" s="1" t="s">
         <v>241</v>
-      </c>
-      <c r="D81" s="1" t="s">
-        <v>242</v>
       </c>
       <c r="E81" s="1" t="s">
         <v>11</v>
@@ -4566,7 +4566,7 @@
         <v>18000</v>
       </c>
       <c r="I81" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J81" s="1"/>
       <c r="K81" s="3">
@@ -4575,22 +4575,22 @@
     </row>
     <row r="82" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A82" s="1" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B82" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C82" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="D82" s="1" t="s">
         <v>244</v>
       </c>
-      <c r="D82" s="1" t="s">
+      <c r="E82" s="1" t="s">
         <v>245</v>
       </c>
-      <c r="E82" s="1" t="s">
+      <c r="F82" s="1" t="s">
         <v>246</v>
-      </c>
-      <c r="F82" s="1" t="s">
-        <v>247</v>
       </c>
       <c r="G82" s="2">
         <v>51000</v>
@@ -4599,7 +4599,7 @@
         <v>34000</v>
       </c>
       <c r="I82" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J82" s="1"/>
       <c r="K82" s="3">
@@ -4608,16 +4608,16 @@
     </row>
     <row r="83" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A83" s="1" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B83" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C83" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="D83" s="1" t="s">
         <v>249</v>
-      </c>
-      <c r="D83" s="1" t="s">
-        <v>250</v>
       </c>
       <c r="E83" s="1" t="s">
         <v>13</v>
@@ -4632,7 +4632,7 @@
         <v>82000</v>
       </c>
       <c r="I83" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="J83" s="1"/>
       <c r="K83" s="3">
@@ -4641,16 +4641,16 @@
     </row>
     <row r="84" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A84" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="B84" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C84" s="1" t="s">
         <v>251</v>
       </c>
-      <c r="B84" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C84" s="1" t="s">
+      <c r="D84" s="1" t="s">
         <v>252</v>
-      </c>
-      <c r="D84" s="1" t="s">
-        <v>253</v>
       </c>
       <c r="E84" s="1" t="s">
         <v>21</v>
@@ -4665,7 +4665,7 @@
         <v>66000</v>
       </c>
       <c r="I84" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="J84" s="1"/>
       <c r="K84" s="3">
@@ -4674,16 +4674,16 @@
     </row>
     <row r="85" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A85" s="1" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B85" s="1" t="s">
         <v>24</v>
       </c>
       <c r="C85" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="D85" s="1" t="s">
         <v>255</v>
-      </c>
-      <c r="D85" s="1" t="s">
-        <v>256</v>
       </c>
       <c r="E85" s="1" t="s">
         <v>13</v>
@@ -4698,7 +4698,7 @@
         <v>80000</v>
       </c>
       <c r="I85" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J85" s="1"/>
       <c r="K85" s="3">
@@ -4707,16 +4707,16 @@
     </row>
     <row r="86" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A86" s="1" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B86" s="1" t="s">
         <v>24</v>
       </c>
       <c r="C86" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="D86" s="1" t="s">
         <v>258</v>
-      </c>
-      <c r="D86" s="1" t="s">
-        <v>259</v>
       </c>
       <c r="E86" s="1" t="s">
         <v>25</v>
@@ -4731,7 +4731,7 @@
         <v>84000</v>
       </c>
       <c r="I86" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J86" s="1"/>
       <c r="K86" s="3">
@@ -4740,16 +4740,16 @@
     </row>
     <row r="87" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A87" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="B87" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C87" s="1" t="s">
         <v>260</v>
       </c>
-      <c r="B87" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="C87" s="1" t="s">
+      <c r="D87" s="1" t="s">
         <v>261</v>
-      </c>
-      <c r="D87" s="1" t="s">
-        <v>262</v>
       </c>
       <c r="E87" s="1" t="s">
         <v>21</v>
@@ -4764,7 +4764,7 @@
         <v>52000</v>
       </c>
       <c r="I87" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="J87" s="1"/>
       <c r="K87" s="3">
@@ -4773,16 +4773,16 @@
     </row>
     <row r="88" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A88" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="B88" s="1" t="s">
         <v>263</v>
       </c>
-      <c r="B88" s="1" t="s">
+      <c r="C88" s="1" t="s">
         <v>264</v>
       </c>
-      <c r="C88" s="1" t="s">
+      <c r="D88" s="1" t="s">
         <v>265</v>
-      </c>
-      <c r="D88" s="1" t="s">
-        <v>266</v>
       </c>
       <c r="E88" s="1" t="s">
         <v>13</v>
@@ -4797,7 +4797,7 @@
         <v>48000</v>
       </c>
       <c r="I88" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="J88" s="1"/>
       <c r="K88" s="3">
@@ -4806,16 +4806,16 @@
     </row>
     <row r="89" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A89" s="1" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B89" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C89" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="D89" s="1" t="s">
         <v>268</v>
-      </c>
-      <c r="D89" s="1" t="s">
-        <v>269</v>
       </c>
       <c r="E89" s="1" t="s">
         <v>25</v>
@@ -4830,7 +4830,7 @@
         <v>50000</v>
       </c>
       <c r="I89" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="J89" s="1"/>
       <c r="K89" s="3">
@@ -4839,16 +4839,16 @@
     </row>
     <row r="90" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A90" s="1" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B90" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C90" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="D90" s="1" t="s">
         <v>271</v>
-      </c>
-      <c r="D90" s="1" t="s">
-        <v>272</v>
       </c>
       <c r="E90" s="1" t="s">
         <v>13</v>
@@ -4863,7 +4863,7 @@
         <v>42000</v>
       </c>
       <c r="I90" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J90" s="1"/>
       <c r="K90" s="3">
@@ -4872,22 +4872,22 @@
     </row>
     <row r="91" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A91" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="B91" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="C91" s="1" t="s">
         <v>273</v>
       </c>
-      <c r="B91" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="C91" s="1" t="s">
+      <c r="D91" s="1" t="s">
         <v>274</v>
       </c>
-      <c r="D91" s="1" t="s">
+      <c r="E91" s="1" t="s">
         <v>275</v>
       </c>
-      <c r="E91" s="1" t="s">
+      <c r="F91" s="1" t="s">
         <v>276</v>
-      </c>
-      <c r="F91" s="1" t="s">
-        <v>277</v>
       </c>
       <c r="G91" s="2">
         <v>42000</v>
@@ -4896,7 +4896,7 @@
         <v>28000</v>
       </c>
       <c r="I91" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="J91" s="1"/>
       <c r="K91" s="3">
@@ -4905,16 +4905,16 @@
     </row>
     <row r="92" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A92" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B92" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C92" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="D92" s="1" t="s">
         <v>279</v>
-      </c>
-      <c r="D92" s="1" t="s">
-        <v>280</v>
       </c>
       <c r="E92" s="1" t="s">
         <v>13</v>
@@ -4929,7 +4929,7 @@
         <v>98000</v>
       </c>
       <c r="I92" s="1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="J92" s="1"/>
       <c r="K92" s="3">
@@ -4938,16 +4938,16 @@
     </row>
     <row r="93" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A93" s="1" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B93" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C93" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="D93" s="1" t="s">
         <v>282</v>
-      </c>
-      <c r="D93" s="1" t="s">
-        <v>283</v>
       </c>
       <c r="E93" s="1" t="s">
         <v>21</v>
@@ -4962,7 +4962,7 @@
         <v>52000</v>
       </c>
       <c r="I93" s="1" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="J93" s="1"/>
       <c r="K93" s="3">
@@ -4971,22 +4971,22 @@
     </row>
     <row r="94" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A94" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="B94" s="1" t="s">
         <v>285</v>
       </c>
-      <c r="B94" s="1" t="s">
+      <c r="C94" s="1" t="s">
         <v>286</v>
       </c>
-      <c r="C94" s="1" t="s">
+      <c r="D94" s="1" t="s">
         <v>287</v>
       </c>
-      <c r="D94" s="1" t="s">
+      <c r="E94" s="1" t="s">
         <v>288</v>
       </c>
-      <c r="E94" s="1" t="s">
+      <c r="F94" s="1" t="s">
         <v>289</v>
-      </c>
-      <c r="F94" s="1" t="s">
-        <v>290</v>
       </c>
       <c r="G94" s="2">
         <v>54000</v>
@@ -4995,7 +4995,7 @@
         <v>36000</v>
       </c>
       <c r="I94" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J94" s="1"/>
       <c r="K94" s="3">
@@ -5004,16 +5004,16 @@
     </row>
     <row r="95" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A95" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="B95" s="1" t="s">
         <v>291</v>
       </c>
-      <c r="B95" s="1" t="s">
+      <c r="C95" s="1" t="s">
         <v>292</v>
       </c>
-      <c r="C95" s="1" t="s">
+      <c r="D95" s="1" t="s">
         <v>293</v>
-      </c>
-      <c r="D95" s="1" t="s">
-        <v>294</v>
       </c>
       <c r="E95" s="1" t="s">
         <v>21</v>
@@ -5028,7 +5028,7 @@
         <v>58000</v>
       </c>
       <c r="I95" s="1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="J95" s="1"/>
       <c r="K95" s="3">
@@ -5037,16 +5037,16 @@
     </row>
     <row r="96" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A96" s="1" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B96" s="1" t="s">
         <v>34</v>
       </c>
       <c r="C96" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="D96" s="1" t="s">
         <v>296</v>
-      </c>
-      <c r="D96" s="1" t="s">
-        <v>297</v>
       </c>
       <c r="E96" s="1" t="s">
         <v>13</v>
@@ -5061,7 +5061,7 @@
         <v>16000</v>
       </c>
       <c r="I96" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J96" s="1"/>
       <c r="K96" s="3">
@@ -5070,19 +5070,19 @@
     </row>
     <row r="97" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A97" s="1" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B97" s="1" t="s">
         <v>31</v>
       </c>
       <c r="C97" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="D97" s="1" t="s">
         <v>299</v>
       </c>
-      <c r="D97" s="1" t="s">
-        <v>300</v>
-      </c>
       <c r="E97" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F97" s="1" t="s">
         <v>32</v>
@@ -5094,7 +5094,7 @@
         <v>44000</v>
       </c>
       <c r="I97" s="1" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="J97" s="1"/>
       <c r="K97" s="3">
@@ -5103,16 +5103,16 @@
     </row>
     <row r="98" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A98" s="1" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B98" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C98" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="D98" s="1" t="s">
         <v>303</v>
-      </c>
-      <c r="D98" s="1" t="s">
-        <v>304</v>
       </c>
       <c r="E98" s="1" t="s">
         <v>13</v>
@@ -5127,7 +5127,7 @@
         <v>84000</v>
       </c>
       <c r="I98" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="J98" s="1"/>
       <c r="K98" s="3">
@@ -5136,22 +5136,22 @@
     </row>
     <row r="99" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A99" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="B99" s="1" t="s">
         <v>305</v>
       </c>
-      <c r="B99" s="1" t="s">
+      <c r="C99" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="D99" s="1" t="s">
         <v>306</v>
       </c>
-      <c r="C99" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="D99" s="1" t="s">
-        <v>307</v>
-      </c>
       <c r="E99" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="F99" s="1" t="s">
         <v>111</v>
-      </c>
-      <c r="F99" s="1" t="s">
-        <v>112</v>
       </c>
       <c r="G99" s="2">
         <v>36000</v>
@@ -5160,7 +5160,7 @@
         <v>24000</v>
       </c>
       <c r="I99" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J99" s="1"/>
       <c r="K99" s="3">
@@ -5169,16 +5169,16 @@
     </row>
     <row r="100" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A100" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="B100" s="1" t="s">
         <v>308</v>
       </c>
-      <c r="B100" s="1" t="s">
+      <c r="C100" s="1" t="s">
         <v>309</v>
       </c>
-      <c r="C100" s="1" t="s">
+      <c r="D100" s="1" t="s">
         <v>310</v>
-      </c>
-      <c r="D100" s="1" t="s">
-        <v>311</v>
       </c>
       <c r="E100" s="1" t="s">
         <v>13</v>
@@ -5193,7 +5193,7 @@
         <v>42000</v>
       </c>
       <c r="I100" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J100" s="1"/>
       <c r="K100" s="3">
@@ -5202,16 +5202,16 @@
     </row>
     <row r="101" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A101" s="1" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B101" s="1" t="s">
         <v>31</v>
       </c>
       <c r="C101" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="D101" s="1" t="s">
         <v>313</v>
-      </c>
-      <c r="D101" s="1" t="s">
-        <v>314</v>
       </c>
       <c r="E101" s="1" t="s">
         <v>13</v>
@@ -5226,7 +5226,7 @@
         <v>70000</v>
       </c>
       <c r="I101" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="J101" s="1"/>
       <c r="K101" s="3">
@@ -5235,16 +5235,16 @@
     </row>
     <row r="102" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A102" s="1" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="B102" s="1" t="s">
         <v>34</v>
       </c>
       <c r="C102" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="D102" s="1" t="s">
         <v>316</v>
-      </c>
-      <c r="D102" s="1" t="s">
-        <v>317</v>
       </c>
       <c r="E102" s="1" t="s">
         <v>13</v>
@@ -5259,7 +5259,7 @@
         <v>54000</v>
       </c>
       <c r="I102" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J102" s="1"/>
       <c r="K102" s="3">
@@ -5268,22 +5268,22 @@
     </row>
     <row r="103" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A103" s="1" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B103" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C103" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="D103" s="1" t="s">
         <v>319</v>
       </c>
-      <c r="D103" s="1" t="s">
+      <c r="E103" s="1" t="s">
         <v>320</v>
       </c>
-      <c r="E103" s="1" t="s">
+      <c r="F103" s="1" t="s">
         <v>321</v>
-      </c>
-      <c r="F103" s="1" t="s">
-        <v>322</v>
       </c>
       <c r="G103" s="2">
         <v>66000</v>
@@ -5292,7 +5292,7 @@
         <v>44000</v>
       </c>
       <c r="I103" s="1" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="J103" s="1"/>
       <c r="K103" s="3">
@@ -5301,22 +5301,22 @@
     </row>
     <row r="104" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A104" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="B104" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="C104" s="1" t="s">
         <v>323</v>
       </c>
-      <c r="B104" s="1" t="s">
-        <v>286</v>
-      </c>
-      <c r="C104" s="1" t="s">
+      <c r="D104" s="1" t="s">
         <v>324</v>
       </c>
-      <c r="D104" s="1" t="s">
-        <v>325</v>
-      </c>
       <c r="E104" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="F104" s="1" t="s">
         <v>289</v>
-      </c>
-      <c r="F104" s="1" t="s">
-        <v>290</v>
       </c>
       <c r="G104" s="2">
         <v>78000</v>
@@ -5325,7 +5325,7 @@
         <v>52000</v>
       </c>
       <c r="I104" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J104" s="1"/>
       <c r="K104" s="3">
@@ -5334,22 +5334,22 @@
     </row>
     <row r="105" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A105" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="B105" s="1" t="s">
         <v>326</v>
       </c>
-      <c r="B105" s="1" t="s">
+      <c r="C105" s="1" t="s">
         <v>327</v>
       </c>
-      <c r="C105" s="1" t="s">
+      <c r="D105" s="1" t="s">
         <v>328</v>
       </c>
-      <c r="D105" s="1" t="s">
-        <v>329</v>
-      </c>
       <c r="E105" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F105" s="1" t="s">
         <v>46</v>
-      </c>
-      <c r="F105" s="1" t="s">
-        <v>47</v>
       </c>
       <c r="G105" s="2">
         <v>375000</v>
@@ -5358,7 +5358,7 @@
         <v>250000</v>
       </c>
       <c r="I105" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="J105" s="1"/>
       <c r="K105" s="3">
@@ -5367,16 +5367,16 @@
     </row>
     <row r="106" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A106" s="1" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B106" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C106" s="1" t="s">
+        <v>330</v>
+      </c>
+      <c r="D106" s="1" t="s">
         <v>331</v>
-      </c>
-      <c r="D106" s="1" t="s">
-        <v>332</v>
       </c>
       <c r="E106" s="1" t="s">
         <v>11</v>
@@ -5391,7 +5391,7 @@
         <v>44000</v>
       </c>
       <c r="I106" s="1" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="J106" s="1"/>
       <c r="K106" s="3">
@@ -5400,29 +5400,29 @@
     </row>
     <row r="107" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A107" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="B107" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="C107" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="D107" s="1" t="s">
         <v>334</v>
       </c>
-      <c r="B107" s="1" t="s">
-        <v>286</v>
-      </c>
-      <c r="C107" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="D107" s="1" t="s">
-        <v>335</v>
-      </c>
       <c r="E107" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="F107" s="1" t="s">
         <v>289</v>
-      </c>
-      <c r="F107" s="1" t="s">
-        <v>290</v>
       </c>
       <c r="G107" s="1"/>
       <c r="H107" s="2">
         <v>12000</v>
       </c>
       <c r="I107" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J107" s="1"/>
       <c r="K107" s="3">
@@ -5431,19 +5431,19 @@
     </row>
     <row r="108" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A108" s="1" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="B108" s="1" t="s">
         <v>27</v>
       </c>
       <c r="C108" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="D108" s="1" t="s">
         <v>337</v>
       </c>
-      <c r="D108" s="1" t="s">
-        <v>338</v>
-      </c>
       <c r="E108" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F108" s="1" t="s">
         <v>32</v>
@@ -5455,7 +5455,7 @@
         <v>84000</v>
       </c>
       <c r="I108" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="J108" s="1"/>
       <c r="K108" s="3">
@@ -5464,22 +5464,22 @@
     </row>
     <row r="109" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A109" s="1" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B109" s="1" t="s">
         <v>24</v>
       </c>
       <c r="C109" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="D109" s="1" t="s">
         <v>340</v>
       </c>
-      <c r="D109" s="1" t="s">
-        <v>341</v>
-      </c>
       <c r="E109" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="F109" s="1" t="s">
         <v>111</v>
-      </c>
-      <c r="F109" s="1" t="s">
-        <v>112</v>
       </c>
       <c r="G109" s="2">
         <v>18000</v>
@@ -5488,7 +5488,7 @@
         <v>12000</v>
       </c>
       <c r="I109" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J109" s="1"/>
       <c r="K109" s="3">
@@ -5497,16 +5497,16 @@
     </row>
     <row r="110" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A110" s="1" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="B110" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C110" s="1" t="s">
+        <v>342</v>
+      </c>
+      <c r="D110" s="1" t="s">
         <v>343</v>
-      </c>
-      <c r="D110" s="1" t="s">
-        <v>344</v>
       </c>
       <c r="E110" s="1" t="s">
         <v>13</v>
@@ -5521,7 +5521,7 @@
         <v>48000</v>
       </c>
       <c r="I110" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J110" s="1"/>
       <c r="K110" s="3">
@@ -5530,16 +5530,16 @@
     </row>
     <row r="111" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A111" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B111" s="1" t="s">
         <v>27</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D111" s="1" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="E111" s="1" t="s">
         <v>5</v>
@@ -5554,7 +5554,7 @@
         <v>34000</v>
       </c>
       <c r="I111" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J111" s="1"/>
       <c r="K111" s="3">
@@ -5563,19 +5563,19 @@
     </row>
     <row r="112" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A112" s="1" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="B112" s="1" t="s">
         <v>33</v>
       </c>
       <c r="C112" s="1" t="s">
+        <v>346</v>
+      </c>
+      <c r="D112" s="1" t="s">
         <v>347</v>
       </c>
-      <c r="D112" s="1" t="s">
-        <v>348</v>
-      </c>
       <c r="E112" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F112" s="1" t="s">
         <v>32</v>
@@ -5587,7 +5587,7 @@
         <v>84000</v>
       </c>
       <c r="I112" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="J112" s="1"/>
       <c r="K112" s="3">
@@ -5596,16 +5596,16 @@
     </row>
     <row r="113" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A113" s="1" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B113" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C113" s="1" t="s">
+        <v>349</v>
+      </c>
+      <c r="D113" s="1" t="s">
         <v>350</v>
-      </c>
-      <c r="D113" s="1" t="s">
-        <v>351</v>
       </c>
       <c r="E113" s="1" t="s">
         <v>11</v>
@@ -5620,7 +5620,7 @@
         <v>38000</v>
       </c>
       <c r="I113" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="J113" s="1"/>
       <c r="K113" s="3">
@@ -5629,16 +5629,16 @@
     </row>
     <row r="114" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A114" s="1" t="s">
+        <v>351</v>
+      </c>
+      <c r="B114" s="1" t="s">
         <v>352</v>
       </c>
-      <c r="B114" s="1" t="s">
+      <c r="C114" s="1" t="s">
         <v>353</v>
       </c>
-      <c r="C114" s="1" t="s">
+      <c r="D114" s="1" t="s">
         <v>354</v>
-      </c>
-      <c r="D114" s="1" t="s">
-        <v>355</v>
       </c>
       <c r="E114" s="1" t="s">
         <v>28</v>
@@ -5653,7 +5653,7 @@
         <v>40000</v>
       </c>
       <c r="I114" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J114" s="1"/>
       <c r="K114" s="3">
@@ -5662,16 +5662,16 @@
     </row>
     <row r="115" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A115" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="B115" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C115" s="1" t="s">
         <v>356</v>
       </c>
-      <c r="B115" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C115" s="1" t="s">
+      <c r="D115" s="1" t="s">
         <v>357</v>
-      </c>
-      <c r="D115" s="1" t="s">
-        <v>358</v>
       </c>
       <c r="E115" s="1" t="s">
         <v>25</v>
@@ -5686,7 +5686,7 @@
         <v>30000</v>
       </c>
       <c r="I115" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J115" s="1"/>
       <c r="K115" s="3">
@@ -5695,16 +5695,16 @@
     </row>
     <row r="116" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A116" s="1" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="B116" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C116" s="1" t="s">
+        <v>359</v>
+      </c>
+      <c r="D116" s="1" t="s">
         <v>360</v>
-      </c>
-      <c r="D116" s="1" t="s">
-        <v>361</v>
       </c>
       <c r="E116" s="1" t="s">
         <v>13</v>
@@ -5719,7 +5719,7 @@
         <v>44000</v>
       </c>
       <c r="I116" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J116" s="1"/>
       <c r="K116" s="3">
@@ -5728,16 +5728,16 @@
     </row>
     <row r="117" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A117" s="1" t="s">
+        <v>361</v>
+      </c>
+      <c r="B117" s="1" t="s">
         <v>362</v>
       </c>
-      <c r="B117" s="1" t="s">
+      <c r="C117" s="1" t="s">
         <v>363</v>
       </c>
-      <c r="C117" s="1" t="s">
+      <c r="D117" s="1" t="s">
         <v>364</v>
-      </c>
-      <c r="D117" s="1" t="s">
-        <v>365</v>
       </c>
       <c r="E117" s="1" t="s">
         <v>25</v>
@@ -5752,7 +5752,7 @@
         <v>110000</v>
       </c>
       <c r="I117" s="1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="J117" s="1"/>
       <c r="K117" s="3">
@@ -5761,16 +5761,16 @@
     </row>
     <row r="118" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A118" s="1" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B118" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C118" s="1" t="s">
+        <v>366</v>
+      </c>
+      <c r="D118" s="1" t="s">
         <v>367</v>
-      </c>
-      <c r="D118" s="1" t="s">
-        <v>368</v>
       </c>
       <c r="E118" s="1" t="s">
         <v>21</v>
@@ -5785,7 +5785,7 @@
         <v>62000</v>
       </c>
       <c r="I118" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="J118" s="1"/>
       <c r="K118" s="3">
@@ -5794,16 +5794,16 @@
     </row>
     <row r="119" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A119" s="1" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="B119" s="1" t="s">
         <v>16</v>
       </c>
       <c r="C119" s="1" t="s">
+        <v>369</v>
+      </c>
+      <c r="D119" s="1" t="s">
         <v>370</v>
-      </c>
-      <c r="D119" s="1" t="s">
-        <v>371</v>
       </c>
       <c r="E119" s="1" t="s">
         <v>13</v>
@@ -5818,7 +5818,7 @@
         <v>90000</v>
       </c>
       <c r="I119" s="1" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="J119" s="1"/>
       <c r="K119" s="3">
@@ -5827,22 +5827,22 @@
     </row>
     <row r="120" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A120" s="1" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="B120" s="1" t="s">
         <v>33</v>
       </c>
       <c r="C120" s="1" t="s">
+        <v>470</v>
+      </c>
+      <c r="D120" s="1" t="s">
         <v>471</v>
       </c>
-      <c r="D120" s="1" t="s">
-        <v>472</v>
-      </c>
       <c r="E120" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="F120" s="1" t="s">
         <v>50</v>
-      </c>
-      <c r="F120" s="1" t="s">
-        <v>51</v>
       </c>
       <c r="G120" s="2">
         <v>6000</v>
@@ -5851,7 +5851,7 @@
         <v>4000</v>
       </c>
       <c r="I120" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J120" s="1"/>
       <c r="K120" s="3">
@@ -5860,16 +5860,16 @@
     </row>
     <row r="121" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A121" s="1" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="B121" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C121" s="1" t="s">
+        <v>473</v>
+      </c>
+      <c r="D121" s="1" t="s">
         <v>474</v>
-      </c>
-      <c r="D121" s="1" t="s">
-        <v>475</v>
       </c>
       <c r="E121" s="1" t="s">
         <v>8</v>
@@ -5884,7 +5884,7 @@
         <v>60000</v>
       </c>
       <c r="I121" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J121" s="1"/>
       <c r="K121" s="3">
@@ -5893,16 +5893,16 @@
     </row>
     <row r="122" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A122" s="1" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="B122" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C122" s="1" t="s">
+        <v>476</v>
+      </c>
+      <c r="D122" s="1" t="s">
         <v>477</v>
-      </c>
-      <c r="D122" s="1" t="s">
-        <v>478</v>
       </c>
       <c r="E122" s="1" t="s">
         <v>13</v>
@@ -5917,7 +5917,7 @@
         <v>52000</v>
       </c>
       <c r="I122" s="1" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="J122" s="1"/>
       <c r="K122" s="3">
@@ -5926,16 +5926,16 @@
     </row>
     <row r="123" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A123" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B123" s="1" t="s">
         <v>15</v>
       </c>
       <c r="C123" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D123" s="1" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="E123" s="1" t="s">
         <v>8</v>
@@ -5950,7 +5950,7 @@
         <v>54000</v>
       </c>
       <c r="I123" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="J123" s="1"/>
       <c r="K123" s="3">
@@ -5959,16 +5959,16 @@
     </row>
     <row r="124" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A124" s="7" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="B124" s="7" t="s">
         <v>17</v>
       </c>
       <c r="C124" s="7" t="s">
+        <v>480</v>
+      </c>
+      <c r="D124" s="7" t="s">
         <v>481</v>
-      </c>
-      <c r="D124" s="7" t="s">
-        <v>482</v>
       </c>
       <c r="E124" s="7" t="s">
         <v>21</v>
@@ -5983,7 +5983,7 @@
         <v>24000</v>
       </c>
       <c r="I124" s="7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J124" s="7"/>
       <c r="K124" s="9">
@@ -5992,22 +5992,22 @@
     </row>
     <row r="125" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A125" s="7" t="s">
+        <v>482</v>
+      </c>
+      <c r="B125" s="7" t="s">
         <v>483</v>
       </c>
-      <c r="B125" s="7" t="s">
+      <c r="C125" s="7" t="s">
         <v>484</v>
       </c>
-      <c r="C125" s="7" t="s">
+      <c r="D125" s="7" t="s">
         <v>485</v>
       </c>
-      <c r="D125" s="7" t="s">
+      <c r="E125" s="7" t="s">
         <v>486</v>
       </c>
-      <c r="E125" s="7" t="s">
+      <c r="F125" s="7" t="s">
         <v>487</v>
-      </c>
-      <c r="F125" s="7" t="s">
-        <v>488</v>
       </c>
       <c r="G125" s="8">
         <v>108000</v>
@@ -6016,7 +6016,7 @@
         <v>72000</v>
       </c>
       <c r="I125" s="7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J125" s="7"/>
       <c r="K125" s="9">
@@ -6025,22 +6025,22 @@
     </row>
     <row r="126" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A126" s="7" t="s">
+        <v>488</v>
+      </c>
+      <c r="B126" s="7" t="s">
         <v>489</v>
       </c>
-      <c r="B126" s="7" t="s">
+      <c r="C126" s="7" t="s">
         <v>490</v>
       </c>
-      <c r="C126" s="7" t="s">
+      <c r="D126" s="7" t="s">
         <v>491</v>
       </c>
-      <c r="D126" s="7" t="s">
+      <c r="E126" s="7" t="s">
         <v>492</v>
       </c>
-      <c r="E126" s="7" t="s">
+      <c r="F126" s="7" t="s">
         <v>493</v>
-      </c>
-      <c r="F126" s="7" t="s">
-        <v>494</v>
       </c>
       <c r="G126" s="8">
         <v>18000</v>
@@ -6049,7 +6049,7 @@
         <v>12000</v>
       </c>
       <c r="I126" s="7" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="J126" s="7"/>
       <c r="K126" s="9">
@@ -6058,16 +6058,16 @@
     </row>
     <row r="127" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A127" s="7" t="s">
+        <v>494</v>
+      </c>
+      <c r="B127" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="C127" s="7" t="s">
         <v>495</v>
       </c>
-      <c r="B127" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="C127" s="7" t="s">
+      <c r="D127" s="7" t="s">
         <v>496</v>
-      </c>
-      <c r="D127" s="7" t="s">
-        <v>497</v>
       </c>
       <c r="E127" s="7" t="s">
         <v>13</v>
@@ -6082,7 +6082,7 @@
         <v>60000</v>
       </c>
       <c r="I127" s="7" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="J127" s="7"/>
       <c r="K127" s="9">
@@ -6091,16 +6091,16 @@
     </row>
     <row r="128" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A128" s="7" t="s">
+        <v>497</v>
+      </c>
+      <c r="B128" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="C128" s="7" t="s">
         <v>498</v>
       </c>
-      <c r="B128" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="C128" s="7" t="s">
+      <c r="D128" s="7" t="s">
         <v>499</v>
-      </c>
-      <c r="D128" s="7" t="s">
-        <v>500</v>
       </c>
       <c r="E128" s="7" t="s">
         <v>13</v>
@@ -6115,7 +6115,7 @@
         <v>32000</v>
       </c>
       <c r="I128" s="7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J128" s="7"/>
       <c r="K128" s="9">
@@ -6124,16 +6124,16 @@
     </row>
     <row r="129" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A129" s="7" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="B129" s="7" t="s">
         <v>7</v>
       </c>
       <c r="C129" s="7" t="s">
+        <v>501</v>
+      </c>
+      <c r="D129" s="7" t="s">
         <v>502</v>
-      </c>
-      <c r="D129" s="7" t="s">
-        <v>503</v>
       </c>
       <c r="E129" s="7" t="s">
         <v>13</v>
@@ -6148,7 +6148,7 @@
         <v>82000</v>
       </c>
       <c r="I129" s="7" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="J129" s="7"/>
       <c r="K129" s="9">

</xml_diff>